<commit_message>
DateType 컬럼 처리 WIP
</commit_message>
<xml_diff>
--- a/src/test/resources/Test13Rows.xlsx
+++ b/src/test/resources/Test13Rows.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="80">
   <si>
     <t>구분</t>
   </si>
@@ -103,9 +103,6 @@
     <t>8801007832265</t>
   </si>
   <si>
-    <t>2022-01-18</t>
-  </si>
-  <si>
     <t>622</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>2021-10-25</t>
-  </si>
-  <si>
     <t>16</t>
   </si>
   <si>
@@ -145,7 +139,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>2021-09-21</t>
+    <t>2021-07-10</t>
   </si>
   <si>
     <t>24</t>
@@ -163,9 +157,6 @@
     <t>8801043032148</t>
   </si>
   <si>
-    <t>2021-07-10</t>
-  </si>
-  <si>
     <t>2021-08-21</t>
   </si>
   <si>
@@ -190,7 +181,7 @@
     <t>A</t>
   </si>
   <si>
-    <t>2021-08-02</t>
+    <t>2021.08.02</t>
   </si>
   <si>
     <t>D101-0302</t>
@@ -205,7 +196,7 @@
     <t>8801007745732</t>
   </si>
   <si>
-    <t>2022-01-21</t>
+    <t>2022/01/21</t>
   </si>
   <si>
     <t>1470</t>
@@ -266,6 +257,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy. M. d"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10.0"/>
@@ -304,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -319,6 +313,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -666,8 +663,8 @@
       <c r="J3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>30</v>
+      <c r="K3" s="5">
+        <v>44579.0</v>
       </c>
       <c r="L3" s="3">
         <v>622.0</v>
@@ -676,7 +673,7 @@
         <v>622.0</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O3" s="4">
         <v>29.0</v>
@@ -691,7 +688,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>18</v>
@@ -700,19 +697,19 @@
         <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>37</v>
+      <c r="K4" s="5">
+        <v>44494.0</v>
       </c>
       <c r="L4" s="3">
         <v>16.0</v>
@@ -721,7 +718,7 @@
         <v>16.0</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O4" s="4">
         <v>2.0</v>
@@ -736,7 +733,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>18</v>
@@ -745,19 +742,19 @@
         <v>19</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="L5" s="3">
         <v>24.0</v>
@@ -766,7 +763,7 @@
         <v>24.0</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O5" s="4">
         <v>4.0</v>
@@ -781,7 +778,7 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>18</v>
@@ -790,19 +787,19 @@
         <v>19</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="L6" s="3">
         <v>22.0</v>
@@ -811,7 +808,7 @@
         <v>22.0</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O6" s="4">
         <v>2.0</v>
@@ -826,7 +823,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>18</v>
@@ -835,19 +832,19 @@
         <v>19</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="J7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="L7" s="3">
         <v>22.0</v>
@@ -856,7 +853,7 @@
         <v>22.0</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O7" s="4">
         <v>2.0</v>
@@ -871,7 +868,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>18</v>
@@ -880,19 +877,19 @@
         <v>19</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="L8" s="3">
         <v>23.0</v>
@@ -901,10 +898,10 @@
         <v>23.0</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
@@ -916,7 +913,7 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>18</v>
@@ -925,19 +922,19 @@
         <v>19</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>59</v>
+        <v>35</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="L9" s="3">
         <v>23.0</v>
@@ -946,7 +943,7 @@
         <v>23.0</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O9" s="4">
         <v>2.0</v>
@@ -961,7 +958,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>18</v>
@@ -970,19 +967,19 @@
         <v>19</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>64</v>
+      <c r="K10" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="L10" s="3">
         <v>1470.0</v>
@@ -991,120 +988,120 @@
         <v>1470.0</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O10" s="4">
         <v>70.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
-        <v>66</v>
+      <c r="A11" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="5" t="s">
-        <v>67</v>
+      <c r="D11" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="K11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="L11" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="M11" s="7">
+        <v>179.0</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L11" s="6">
-        <v>1.0</v>
-      </c>
-      <c r="M11" s="6">
-        <v>179.0</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="O11" s="4"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
-        <v>66</v>
+      <c r="A12" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="5" t="s">
-        <v>67</v>
+      <c r="D12" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="L12" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="M12" s="7">
+        <v>179.0</v>
+      </c>
+      <c r="N12" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="L12" s="6">
-        <v>2.0</v>
-      </c>
-      <c r="M12" s="6">
-        <v>179.0</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="O12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
-        <v>66</v>
+      <c r="A13" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="5" t="s">
-        <v>67</v>
+      <c r="D13" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="L13" s="6">
+      <c r="L13" s="7">
         <v>1.0</v>
       </c>
-      <c r="M13" s="6">
+      <c r="M13" s="7">
         <v>179.0</v>
       </c>
-      <c r="N13" s="5" t="s">
-        <v>73</v>
+      <c r="N13" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="O13" s="4"/>
     </row>

</xml_diff>